<commit_message>
Co-authored-by: Sahishnu Hanumolu <Sahish08@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/inputs/portfolio1/portfolio_data.xlsx
+++ b/inputs/portfolio1/portfolio_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>symbol</t>
   </si>
@@ -31,6 +31,9 @@
     <t>sector</t>
   </si>
   <si>
+    <t>asset_type</t>
+  </si>
+  <si>
     <t>AAPL</t>
   </si>
   <si>
@@ -143,6 +146,9 @@
   </si>
   <si>
     <t>Consumer Staples</t>
+  </si>
+  <si>
+    <t>Stock</t>
   </si>
 </sst>
 </file>
@@ -500,13 +506,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,277 +528,328 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>150</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D3">
         <v>250</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4">
         <v>2800</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>400</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6">
         <v>320</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>150</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7">
         <v>220</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8">
         <v>200</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9">
         <v>300</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>140</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>120</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D11">
         <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D12">
         <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13">
         <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14">
         <v>160</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>42</v>
+      </c>
+      <c r="F14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D15">
         <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D16">
         <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D17">
         <v>150</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>